<commit_message>
checked if script for growth is correct found small issue with joins as sometimes data are present in HBI but not in BZE3, as all our joins are based on BZE3 present data/ categories/ groups, this leads to NAs in case of deadwood compartiments, regeneration compartiments and living trees species
</commit_message>
<xml_diff>
--- a/playground/example_output_ha_all_groups.xlsx
+++ b/playground/example_output_ha_all_groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gercken\Documents\TI_BZE_BE_analysis\playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78301B6C-7AC8-4762-A72F-602CAFAF4031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172793FE-0433-4D20-98DB-D1596C1322FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -877,18 +877,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z11" sqref="Z11"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1796875" style="21"/>
+    <col min="2" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>53</v>
       </c>
@@ -980,7 +980,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="22"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -1073,7 +1073,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>33</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="24"/>
       <c r="B4" s="8" t="s">
         <v>15</v>
@@ -1261,7 +1261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="24"/>
       <c r="B5" s="8" t="s">
         <v>15</v>
@@ -1354,7 +1354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="8" t="s">
         <v>15</v>
@@ -1447,7 +1447,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="8" t="s">
         <v>15</v>
@@ -1540,7 +1540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="8" t="s">
         <v>15</v>
@@ -1633,7 +1633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="8" t="s">
         <v>15</v>
@@ -1726,7 +1726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="8" t="s">
         <v>15</v>
@@ -1819,7 +1819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25"/>
       <c r="B11" s="11" t="s">
         <v>15</v>
@@ -1912,7 +1912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>31</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="8" t="s">
         <v>15</v>
@@ -2100,7 +2100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" s="27"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
@@ -2193,7 +2193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="27"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
@@ -2286,7 +2286,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="27"/>
       <c r="B16" s="8" t="s">
         <v>15</v>
@@ -2379,7 +2379,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" s="27"/>
       <c r="B17" s="8" t="s">
         <v>15</v>
@@ -2472,7 +2472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" s="27"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
@@ -2565,7 +2565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="8" t="s">
         <v>15</v>
@@ -2658,7 +2658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="B20" s="11" t="s">
         <v>15</v>
@@ -2751,7 +2751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>32</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
@@ -2939,7 +2939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
       <c r="B23" s="8" t="s">
         <v>15</v>
@@ -3032,7 +3032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="8" t="s">
         <v>15</v>
@@ -3125,7 +3125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="8" t="s">
         <v>15</v>
@@ -3218,7 +3218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="B26" s="8" t="s">
         <v>15</v>
@@ -3311,7 +3311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" s="24"/>
       <c r="B27" s="8" t="s">
         <v>15</v>
@@ -3404,7 +3404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A28" s="24"/>
       <c r="B28" s="8" t="s">
         <v>15</v>
@@ -3497,7 +3497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25"/>
       <c r="B29" s="11" t="s">
         <v>15</v>
@@ -3590,7 +3590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>34</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31" s="24"/>
       <c r="B31" s="8" t="s">
         <v>15</v>
@@ -3778,7 +3778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32" s="24"/>
       <c r="B32" s="8" t="s">
         <v>15</v>
@@ -3871,7 +3871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A33" s="24"/>
       <c r="B33" s="8" t="s">
         <v>15</v>
@@ -3964,7 +3964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A34" s="24"/>
       <c r="B34" s="8" t="s">
         <v>15</v>
@@ -4057,7 +4057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A35" s="24"/>
       <c r="B35" s="8" t="s">
         <v>15</v>
@@ -4150,7 +4150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A36" s="24"/>
       <c r="B36" s="8" t="s">
         <v>15</v>
@@ -4243,7 +4243,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A37" s="24"/>
       <c r="B37" s="8" t="s">
         <v>15</v>
@@ -4336,7 +4336,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="25"/>
       <c r="B38" s="11" t="s">
         <v>15</v>
@@ -4429,7 +4429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A39" s="26" t="s">
         <v>41</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A40" s="27"/>
       <c r="B40" s="8" t="s">
         <v>15</v>
@@ -4617,7 +4617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A41" s="27"/>
       <c r="B41" s="8" t="s">
         <v>15</v>
@@ -4710,7 +4710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A42" s="27"/>
       <c r="B42" s="8" t="s">
         <v>15</v>
@@ -4803,7 +4803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A43" s="27"/>
       <c r="B43" s="8" t="s">
         <v>15</v>
@@ -4896,7 +4896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A44" s="27"/>
       <c r="B44" s="8" t="s">
         <v>15</v>
@@ -4989,7 +4989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A45" s="27"/>
       <c r="B45" s="8" t="s">
         <v>15</v>
@@ -5082,7 +5082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A46" s="27"/>
       <c r="B46" s="8" t="s">
         <v>15</v>
@@ -5175,7 +5175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="28"/>
       <c r="B47" s="11" t="s">
         <v>15</v>
@@ -5268,7 +5268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A48" s="23" t="s">
         <v>35</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A49" s="24"/>
       <c r="B49" s="8" t="s">
         <v>26</v>
@@ -5456,7 +5456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A50" s="24"/>
       <c r="B50" s="8" t="s">
         <v>26</v>
@@ -5549,7 +5549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A51" s="24"/>
       <c r="B51" s="8" t="s">
         <v>26</v>
@@ -5642,7 +5642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A52" s="24"/>
       <c r="B52" s="8" t="s">
         <v>26</v>
@@ -5735,7 +5735,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A53" s="24"/>
       <c r="B53" s="8" t="s">
         <v>26</v>
@@ -5828,7 +5828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A54" s="24"/>
       <c r="B54" s="8" t="s">
         <v>26</v>
@@ -5921,7 +5921,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A55" s="24"/>
       <c r="B55" s="8" t="s">
         <v>26</v>
@@ -6014,7 +6014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A56" s="24"/>
       <c r="B56" s="8" t="s">
         <v>26</v>
@@ -6107,7 +6107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A57" s="24"/>
       <c r="B57" s="8" t="s">
         <v>26</v>
@@ -6200,7 +6200,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="25"/>
       <c r="B58" s="11" t="s">
         <v>26</v>
@@ -6293,7 +6293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A59" s="23" t="s">
         <v>36</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A60" s="24"/>
       <c r="B60" s="8" t="s">
         <v>26</v>
@@ -6481,7 +6481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A61" s="24"/>
       <c r="B61" s="8" t="s">
         <v>26</v>
@@ -6574,7 +6574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A62" s="24"/>
       <c r="B62" s="8" t="s">
         <v>26</v>
@@ -6667,7 +6667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A63" s="24"/>
       <c r="B63" s="8" t="s">
         <v>26</v>
@@ -6760,7 +6760,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A64" s="24"/>
       <c r="B64" s="8" t="s">
         <v>26</v>
@@ -6853,7 +6853,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A65" s="24"/>
       <c r="B65" s="8" t="s">
         <v>26</v>
@@ -6946,7 +6946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A66" s="24"/>
       <c r="B66" s="8" t="s">
         <v>26</v>
@@ -7039,7 +7039,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A67" s="24"/>
       <c r="B67" s="8" t="s">
         <v>26</v>
@@ -7132,7 +7132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A68" s="24"/>
       <c r="B68" s="8" t="s">
         <v>26</v>
@@ -7225,7 +7225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="25"/>
       <c r="B69" s="11" t="s">
         <v>26</v>
@@ -7318,7 +7318,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A70" s="23" t="s">
         <v>36</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A71" s="24"/>
       <c r="B71" s="8" t="s">
         <v>26</v>
@@ -7506,7 +7506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A72" s="24"/>
       <c r="B72" s="8" t="s">
         <v>26</v>
@@ -7599,7 +7599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A73" s="24"/>
       <c r="B73" s="8" t="s">
         <v>26</v>
@@ -7692,7 +7692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="25"/>
       <c r="B74" s="11" t="s">
         <v>26</v>
@@ -7785,7 +7785,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A75" s="23" t="s">
         <v>37</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A76" s="24"/>
       <c r="B76" s="8" t="s">
         <v>26</v>
@@ -7973,7 +7973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A77" s="24"/>
       <c r="B77" s="8" t="s">
         <v>26</v>
@@ -8066,7 +8066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A78" s="24"/>
       <c r="B78" s="8" t="s">
         <v>26</v>
@@ -8159,7 +8159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="25"/>
       <c r="B79" s="11" t="s">
         <v>26</v>
@@ -8252,7 +8252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A80" s="23" t="s">
         <v>40</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A81" s="24"/>
       <c r="B81" s="8" t="s">
         <v>29</v>
@@ -8440,7 +8440,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A82" s="24"/>
       <c r="B82" s="8" t="s">
         <v>29</v>
@@ -8533,7 +8533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A83" s="24"/>
       <c r="B83" s="8" t="s">
         <v>29</v>
@@ -8626,7 +8626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A84" s="24"/>
       <c r="B84" s="8" t="s">
         <v>29</v>
@@ -8719,7 +8719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A85" s="24"/>
       <c r="B85" s="8" t="s">
         <v>29</v>
@@ -8812,7 +8812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A86" s="24"/>
       <c r="B86" s="8" t="s">
         <v>29</v>
@@ -8905,7 +8905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A87" s="24"/>
       <c r="B87" s="8" t="s">
         <v>29</v>
@@ -8998,7 +8998,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="25"/>
       <c r="B88" s="11" t="s">
         <v>29</v>
@@ -9091,7 +9091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A89" s="23" t="s">
         <v>39</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A90" s="24"/>
       <c r="B90" s="8" t="s">
         <v>29</v>
@@ -9279,7 +9279,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A91" s="24"/>
       <c r="B91" s="8" t="s">
         <v>29</v>
@@ -9372,7 +9372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="25"/>
       <c r="B92" s="11" t="s">
         <v>29</v>
@@ -9465,7 +9465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A93" s="23" t="s">
         <v>38</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A94" s="24"/>
       <c r="B94" s="8" t="s">
         <v>29</v>
@@ -9653,7 +9653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A95" s="24"/>
       <c r="B95" s="8" t="s">
         <v>29</v>
@@ -9746,7 +9746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A96" s="24"/>
       <c r="B96" s="8" t="s">
         <v>29</v>
@@ -9839,7 +9839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A97" s="24"/>
       <c r="B97" s="8" t="s">
         <v>29</v>
@@ -9932,7 +9932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="25"/>
       <c r="B98" s="11" t="s">
         <v>29</v>
@@ -10025,7 +10025,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A99" s="23" t="s">
         <v>42</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A100" s="24"/>
       <c r="B100" s="8" t="s">
         <v>29</v>
@@ -10213,7 +10213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A101" s="24"/>
       <c r="B101" s="8" t="s">
         <v>29</v>
@@ -10306,7 +10306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A102" s="24"/>
       <c r="B102" s="8" t="s">
         <v>29</v>
@@ -10399,7 +10399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A103" s="24"/>
       <c r="B103" s="8" t="s">
         <v>29</v>
@@ -10492,7 +10492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A104" s="24"/>
       <c r="B104" s="8" t="s">
         <v>29</v>
@@ -10585,7 +10585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A105" s="24"/>
       <c r="B105" s="8" t="s">
         <v>29</v>
@@ -10678,7 +10678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A106" s="24"/>
       <c r="B106" s="8" t="s">
         <v>29</v>
@@ -10771,7 +10771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="25"/>
       <c r="B107" s="11" t="s">
         <v>29</v>
@@ -10864,7 +10864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A108" s="23" t="s">
         <v>44</v>
       </c>
@@ -10959,7 +10959,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A109" s="24"/>
       <c r="B109" s="8" t="s">
         <v>29</v>
@@ -11052,7 +11052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A110" s="24"/>
       <c r="B110" s="8" t="s">
         <v>29</v>
@@ -11145,7 +11145,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="25"/>
       <c r="B111" s="11" t="s">
         <v>29</v>
@@ -11238,7 +11238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A112" s="23" t="s">
         <v>45</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A113" s="24"/>
       <c r="B113" s="8" t="s">
         <v>29</v>
@@ -11426,7 +11426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A114" s="24"/>
       <c r="B114" s="8" t="s">
         <v>29</v>
@@ -11519,7 +11519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A115" s="24"/>
       <c r="B115" s="8" t="s">
         <v>29</v>
@@ -11612,7 +11612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A116" s="24"/>
       <c r="B116" s="8" t="s">
         <v>29</v>
@@ -11705,7 +11705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="25"/>
       <c r="B117" s="11" t="s">
         <v>29</v>
@@ -11798,7 +11798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A118" s="23" t="s">
         <v>46</v>
       </c>
@@ -11893,7 +11893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A119" s="24"/>
       <c r="B119" s="8" t="s">
         <v>29</v>
@@ -11986,7 +11986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="25"/>
       <c r="B120" s="11" t="s">
         <v>29</v>
@@ -12079,7 +12079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A121" s="23" t="s">
         <v>47</v>
       </c>
@@ -12174,7 +12174,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A122" s="24"/>
       <c r="B122" s="8" t="s">
         <v>29</v>
@@ -12267,7 +12267,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A123" s="25"/>
       <c r="B123" s="11" t="s">
         <v>29</v>
@@ -12360,7 +12360,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A124" s="23" t="s">
         <v>43</v>
       </c>
@@ -12455,7 +12455,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A125" s="24"/>
       <c r="B125" s="8" t="s">
         <v>13</v>
@@ -12548,7 +12548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A126" s="25"/>
       <c r="B126" s="11" t="s">
         <v>13</v>
@@ -12641,16 +12641,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A127" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="A48:A58"/>
     <mergeCell ref="A118:A120"/>
     <mergeCell ref="A121:A123"/>
     <mergeCell ref="A124:A126"/>
@@ -12664,6 +12659,11 @@
     <mergeCell ref="A89:A92"/>
     <mergeCell ref="A59:A69"/>
     <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="A48:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>